<commit_message>
Feature: Download report xlsx with chosen export criteria
</commit_message>
<xml_diff>
--- a/bin/constants/ReportTemplate.xlsx
+++ b/bin/constants/ReportTemplate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VehicleParts\server\bin\constants\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{794EFE3B-A99C-4E15-8F86-26496CBDF3B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF2648C2-C132-4174-89E3-B360A8198B4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Parts" sheetId="1" r:id="rId1"/>
@@ -66,21 +66,15 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF00B0F0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -103,22 +97,40 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -401,44 +413,53 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="F1" activeCellId="2" sqref="D1:D1048576 E1:E1048576 F1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.109375" style="3" customWidth="1"/>
-    <col min="2" max="2" width="33.33203125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="25.5546875" style="3" customWidth="1"/>
-    <col min="4" max="5" width="13.33203125" style="3" customWidth="1"/>
-    <col min="6" max="6" width="25" style="3" customWidth="1"/>
-    <col min="7" max="8" width="8.88671875" style="3" customWidth="1"/>
-    <col min="9" max="16384" width="8.88671875" style="3"/>
+    <col min="1" max="1" width="21.109375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="33.33203125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="25.5546875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="7.21875" style="7" customWidth="1"/>
+    <col min="5" max="5" width="8.88671875" style="7" customWidth="1"/>
+    <col min="6" max="6" width="13.88671875" style="7" customWidth="1"/>
+    <col min="7" max="8" width="8.88671875" style="2" customWidth="1"/>
+    <col min="9" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" s="5"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+    </row>
+    <row r="2" spans="1:8" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>